<commit_message>
refactor: caminho da planilha excel para uma variavel de ambiente e adiocionando requirements.txt
</commit_message>
<xml_diff>
--- a/Integração, ASO e Certificados -Terceiros - Atualizada.xlsx
+++ b/Integração, ASO e Certificados -Terceiros - Atualizada.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livia.brito\Desktop\Terceiros.python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livia.brito\Desktop\controle_terceiros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAC6458-1EFD-4424-B698-DBCDC8C08BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D2A061-3C51-4E01-9DD6-A9E260A21D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="29040" windowHeight="15720" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -5368,7 +5368,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6553,7 +6553,7 @@
       </c>
       <c r="I9" s="24" t="str">
         <f ca="1">IFERROR(IF(G9="","?",IF((G9+(365))&lt;TODAY(),"Vencido",IF((G9+(365))=TODAY(),"Vence Hoje",IF((G9+(365)-15)&lt;=TODAY(),"Vence - 15 dias",IF((G9+(365)-30)&lt;=TODAY(),"Vence - 30 dias",IF((G9+(365)-60)&lt;=TODAY(),"Vence - 60 dias",IF((G9+(365)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>41</v>
@@ -6680,7 +6680,7 @@
       </c>
       <c r="I10" s="24" t="str">
         <f ca="1">IFERROR(IF(G10="","?",IF((G10+(365))&lt;TODAY(),"Vencido",IF((G10+(365))=TODAY(),"Vence Hoje",IF((G10+(365)-15)&lt;=TODAY(),"Vence - 15 dias",IF((G10+(365)-30)&lt;=TODAY(),"Vence - 30 dias",IF((G10+(365)-60)&lt;=TODAY(),"Vence - 60 dias",IF((G10+(365)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J10" s="24" t="s">
         <v>41</v>
@@ -6710,7 +6710,7 @@
       </c>
       <c r="R10" s="47" t="str">
         <f t="shared" ref="R10:R21" ca="1" si="5">IFERROR(IF(Q10="","?",IF((Q10+(365*5))&lt;TODAY(),"Vencido",IF((Q10+(365*5))=TODAY(),"Vence Hoje",IF((Q10+(365*5)-15)&lt;=TODAY(),"Vence - 15 dias",IF((Q10+(365*5)-30)&lt;=TODAY(),"Vence - 30 dias",IF((Q10+(365*5)-60)&lt;=TODAY(),"Vence - 60 dias",IF((Q10+(365*5)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="S10" s="40"/>
       <c r="T10" s="40" t="s">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="I16" s="24" t="str">
         <f t="shared" ref="I16:I21" ca="1" si="7">IFERROR(IF(G16="","?",IF((G16+(365))&lt;TODAY(),"Vencido",IF((G16+(365))=TODAY(),"Vence Hoje",IF((G16+(365)-15)&lt;=TODAY(),"Vence - 15 dias",IF((G16+(365)-30)&lt;=TODAY(),"Vence - 30 dias",IF((G16+(365)-60)&lt;=TODAY(),"Vence - 60 dias",IF((G16+(365)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J16" s="24" t="s">
         <v>41</v>
@@ -8170,7 +8170,7 @@
       </c>
       <c r="I17" s="24" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Vence - 60 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J17" s="24" t="s">
         <v>41</v>
@@ -9566,7 +9566,7 @@
       </c>
       <c r="O26" s="46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P26" s="46" t="s">
         <v>42</v>
@@ -10010,7 +10010,7 @@
       </c>
       <c r="O28" s="46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P28" s="46" t="s">
         <v>42</v>
@@ -14909,7 +14909,7 @@
       </c>
       <c r="I54" s="24" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J54" s="24" t="s">
         <v>41</v>
@@ -16431,7 +16431,7 @@
       </c>
       <c r="I61" s="24" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J61" s="24" t="s">
         <v>41</v>
@@ -17586,7 +17586,7 @@
       </c>
       <c r="I66" s="24" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J66" s="24" t="s">
         <v>41</v>
@@ -22455,7 +22455,7 @@
       </c>
       <c r="O99" s="46" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P99" s="46" t="s">
         <v>42</v>
@@ -23188,7 +23188,7 @@
       </c>
       <c r="AF105" s="22" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AG105" s="45"/>
       <c r="AH105" s="45"/>
@@ -23347,7 +23347,7 @@
       </c>
       <c r="I107" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J107" s="24" t="s">
         <v>41</v>
@@ -23427,14 +23427,14 @@
       </c>
       <c r="AJ107" s="22" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AK107" s="33">
         <v>45536</v>
       </c>
       <c r="AL107" s="25" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AM107" s="60"/>
       <c r="AN107" s="40"/>
@@ -23467,7 +23467,7 @@
       </c>
       <c r="I108" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J108" s="24" t="s">
         <v>41</v>
@@ -23547,14 +23547,14 @@
       </c>
       <c r="AJ108" s="22" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AK108" s="33">
         <v>45536</v>
       </c>
       <c r="AL108" s="25" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AM108" s="60"/>
       <c r="AN108" s="40"/>
@@ -23587,7 +23587,7 @@
       </c>
       <c r="I109" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J109" s="24" t="s">
         <v>41</v>
@@ -23667,14 +23667,14 @@
       </c>
       <c r="AJ109" s="22" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AK109" s="33">
         <v>45536</v>
       </c>
       <c r="AL109" s="25" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AM109" s="60"/>
       <c r="AN109" s="40"/>
@@ -23707,7 +23707,7 @@
       </c>
       <c r="I110" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J110" s="24" t="s">
         <v>41</v>
@@ -23787,14 +23787,14 @@
       </c>
       <c r="AJ110" s="22" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AK110" s="33">
         <v>45536</v>
       </c>
       <c r="AL110" s="25" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AM110" s="60"/>
       <c r="AN110" s="40"/>
@@ -23827,7 +23827,7 @@
       </c>
       <c r="I111" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J111" s="24" t="s">
         <v>41</v>
@@ -23907,14 +23907,14 @@
       </c>
       <c r="AJ111" s="22" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AK111" s="33">
         <v>45536</v>
       </c>
       <c r="AL111" s="25" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AM111" s="60"/>
       <c r="AN111" s="40"/>
@@ -23947,7 +23947,7 @@
       </c>
       <c r="I112" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J112" s="24" t="s">
         <v>41</v>
@@ -24027,14 +24027,14 @@
       </c>
       <c r="AJ112" s="22" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AK112" s="33">
         <v>45536</v>
       </c>
       <c r="AL112" s="25" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AM112" s="60"/>
       <c r="AN112" s="40"/>
@@ -24396,7 +24396,7 @@
       </c>
       <c r="AL115" s="25" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AM115" s="40" t="s">
         <v>85</v>
@@ -24433,7 +24433,7 @@
       </c>
       <c r="I116" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J116" s="21" t="s">
         <v>41</v>
@@ -24518,7 +24518,7 @@
       </c>
       <c r="AL116" s="25" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AM116" s="40" t="s">
         <v>85</v>
@@ -24696,7 +24696,7 @@
       </c>
       <c r="O117" s="46" t="str">
         <f t="shared" ref="O117:O180" ca="1" si="26">IFERROR(IF(M117="","?",IF((M117+(365))&lt;TODAY(),"Bloqueado",IF((M117+(365*2))=TODAY(),"Vence Hoje",IF((M117+(365*2)-15)&lt;=TODAY(),"Vence - 15 dias",IF((M117+(365*2)-30)&lt;=TODAY(),"Vence - 30 dias",IF((M117+(365*2)-60)&lt;=TODAY(),"Vence - 60 dias",IF((M117+(365*2)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P117" s="46" t="s">
         <v>42</v>
@@ -24763,7 +24763,7 @@
       </c>
       <c r="AL117" s="25" t="str">
         <f t="shared" ref="AL117:AL180" ca="1" si="27">IFERROR(IF(AK117="","?",IF((AK117+(365))&lt;TODAY(),"Vencido",IF((AK117+(365))=TODAY(),"Vence Hoje",IF((AK117+(365)-15)&lt;=TODAY(),"Vence - 15 dias",IF((AK117+(365)-30)&lt;=TODAY(),"Vence - 30 dias",IF((AK117+(365)-60)&lt;=TODAY(),"Vence - 60 dias",IF((AK117+(365)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AM117" s="40" t="s">
         <v>85</v>
@@ -25008,7 +25008,7 @@
       </c>
       <c r="AL118" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AM118" s="40" t="s">
         <v>85</v>
@@ -25135,7 +25135,7 @@
       </c>
       <c r="AL119" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AM119" s="40" t="s">
         <v>85</v>
@@ -25172,7 +25172,7 @@
       </c>
       <c r="I120" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J120" s="21" t="s">
         <v>41</v>
@@ -25260,7 +25260,7 @@
       </c>
       <c r="AL120" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AM120" s="60" t="s">
         <v>61</v>
@@ -25817,7 +25817,7 @@
       </c>
       <c r="I125" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J125" s="24" t="s">
         <v>41</v>
@@ -26061,7 +26061,7 @@
       </c>
       <c r="I127" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J127" s="24" t="s">
         <v>60</v>
@@ -27199,7 +27199,7 @@
       </c>
       <c r="I136" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J136" s="24" t="s">
         <v>60</v>
@@ -27705,7 +27705,7 @@
       </c>
       <c r="I140" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J140" s="24" t="s">
         <v>60</v>
@@ -27832,7 +27832,7 @@
       </c>
       <c r="I141" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J141" s="24" t="s">
         <v>41</v>
@@ -27959,7 +27959,7 @@
       </c>
       <c r="I142" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J142" s="24" t="s">
         <v>60</v>
@@ -28029,7 +28029,7 @@
       </c>
       <c r="AF142" s="22" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>Vence - 90 dias</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="AG142" s="45" t="s">
         <v>85</v>
@@ -28400,7 +28400,7 @@
       </c>
       <c r="AF145" s="22" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>Vence - 90 dias</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="AG145" s="45" t="s">
         <v>61</v>
@@ -28584,7 +28584,7 @@
       </c>
       <c r="I147" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J147" s="20" t="s">
         <v>41</v>
@@ -28671,7 +28671,7 @@
       </c>
       <c r="AL147" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM147" s="60" t="s">
         <v>61</v>
@@ -28708,7 +28708,7 @@
       </c>
       <c r="I148" s="24" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J148" s="24" t="s">
         <v>41</v>
@@ -28728,7 +28728,7 @@
       </c>
       <c r="O148" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P148" s="46" t="s">
         <v>42</v>
@@ -28795,7 +28795,7 @@
       </c>
       <c r="AL148" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM148" s="60" t="s">
         <v>61</v>
@@ -29218,7 +29218,7 @@
       </c>
       <c r="O152" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P152" s="46" t="s">
         <v>42</v>
@@ -29586,7 +29586,7 @@
       </c>
       <c r="O155" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P155" s="46" t="s">
         <v>42</v>
@@ -31421,7 +31421,7 @@
       </c>
       <c r="I170" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J170" s="20" t="s">
         <v>60</v>
@@ -31544,7 +31544,7 @@
       </c>
       <c r="I171" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J171" s="24" t="s">
         <v>60</v>
@@ -31564,7 +31564,7 @@
       </c>
       <c r="O171" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P171" s="46" t="s">
         <v>42</v>
@@ -31629,7 +31629,7 @@
       </c>
       <c r="AL171" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM171" s="60" t="s">
         <v>84</v>
@@ -31686,7 +31686,7 @@
       </c>
       <c r="O172" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P172" s="46" t="s">
         <v>42</v>
@@ -31751,7 +31751,7 @@
       </c>
       <c r="AL172" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM172" s="60" t="s">
         <v>84</v>
@@ -31808,7 +31808,7 @@
       </c>
       <c r="O173" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P173" s="46" t="s">
         <v>42</v>
@@ -31873,7 +31873,7 @@
       </c>
       <c r="AL173" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM173" s="60" t="s">
         <v>84</v>
@@ -31930,7 +31930,7 @@
       </c>
       <c r="O174" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P174" s="46" t="s">
         <v>42</v>
@@ -31995,7 +31995,7 @@
       </c>
       <c r="AL174" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM174" s="60" t="s">
         <v>84</v>
@@ -32052,7 +32052,7 @@
       </c>
       <c r="O175" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P175" s="46" t="s">
         <v>42</v>
@@ -32117,7 +32117,7 @@
       </c>
       <c r="AL175" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM175" s="60" t="s">
         <v>84</v>
@@ -32154,7 +32154,7 @@
       </c>
       <c r="I176" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J176" s="24" t="s">
         <v>60</v>
@@ -32174,7 +32174,7 @@
       </c>
       <c r="O176" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P176" s="46" t="s">
         <v>42</v>
@@ -32239,7 +32239,7 @@
       </c>
       <c r="AL176" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM176" s="60" t="s">
         <v>90</v>
@@ -32276,7 +32276,7 @@
       </c>
       <c r="I177" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J177" s="21" t="s">
         <v>341</v>
@@ -32359,7 +32359,7 @@
       </c>
       <c r="AL177" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM177" s="60" t="s">
         <v>85</v>
@@ -32396,7 +32396,7 @@
       </c>
       <c r="I178" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J178" s="24" t="s">
         <v>41</v>
@@ -32416,7 +32416,7 @@
       </c>
       <c r="O178" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P178" s="46" t="s">
         <v>42</v>
@@ -32481,7 +32481,7 @@
       </c>
       <c r="AL178" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM178" s="60" t="s">
         <v>84</v>
@@ -32538,7 +32538,7 @@
       </c>
       <c r="O179" s="46" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P179" s="46" t="s">
         <v>42</v>
@@ -32603,7 +32603,7 @@
       </c>
       <c r="AL179" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM179" s="60" t="s">
         <v>84</v>
@@ -32725,7 +32725,7 @@
       </c>
       <c r="AL180" s="25" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM180" s="60" t="s">
         <v>84</v>
@@ -32845,7 +32845,7 @@
       </c>
       <c r="AL181" s="25" t="str">
         <f t="shared" ref="AL181:AL244" ca="1" si="41">IFERROR(IF(AK181="","?",IF((AK181+(365))&lt;TODAY(),"Vencido",IF((AK181+(365))=TODAY(),"Vence Hoje",IF((AK181+(365)-15)&lt;=TODAY(),"Vence - 15 dias",IF((AK181+(365)-30)&lt;=TODAY(),"Vence - 30 dias",IF((AK181+(365)-60)&lt;=TODAY(),"Vence - 60 dias",IF((AK181+(365)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM181" s="60" t="s">
         <v>84</v>
@@ -32902,7 +32902,7 @@
       </c>
       <c r="O182" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P182" s="46" t="s">
         <v>42</v>
@@ -32967,7 +32967,7 @@
       </c>
       <c r="AL182" s="25" t="str">
         <f t="shared" ca="1" si="41"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM182" s="60" t="s">
         <v>84</v>
@@ -33024,7 +33024,7 @@
       </c>
       <c r="O183" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P183" s="46" t="s">
         <v>42</v>
@@ -33089,7 +33089,7 @@
       </c>
       <c r="AL183" s="25" t="str">
         <f t="shared" ca="1" si="41"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM183" s="60" t="s">
         <v>85</v>
@@ -33146,7 +33146,7 @@
       </c>
       <c r="O184" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P184" s="46" t="s">
         <v>42</v>
@@ -33211,7 +33211,7 @@
       </c>
       <c r="AL184" s="25" t="str">
         <f t="shared" ca="1" si="41"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM184" s="60" t="s">
         <v>85</v>
@@ -33764,7 +33764,7 @@
       </c>
       <c r="O189" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P189" s="46" t="s">
         <v>42</v>
@@ -33829,7 +33829,7 @@
       </c>
       <c r="AL189" s="25" t="str">
         <f t="shared" ca="1" si="41"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AM189" s="60" t="s">
         <v>61</v>
@@ -33866,7 +33866,7 @@
       </c>
       <c r="I190" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J190" s="24" t="s">
         <v>60</v>
@@ -33988,7 +33988,7 @@
       </c>
       <c r="I191" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J191" s="24" t="s">
         <v>60</v>
@@ -34110,7 +34110,7 @@
       </c>
       <c r="I192" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J192" s="24" t="s">
         <v>60</v>
@@ -34378,7 +34378,7 @@
       </c>
       <c r="O194" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P194" s="46" t="s">
         <v>42</v>
@@ -34476,7 +34476,7 @@
       </c>
       <c r="I195" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J195" s="24" t="s">
         <v>41</v>
@@ -34496,7 +34496,7 @@
       </c>
       <c r="O195" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P195" s="46" t="s">
         <v>42</v>
@@ -34596,7 +34596,7 @@
       </c>
       <c r="I196" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J196" s="24" t="s">
         <v>41</v>
@@ -34616,7 +34616,7 @@
       </c>
       <c r="O196" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P196" s="46" t="s">
         <v>42</v>
@@ -34834,7 +34834,7 @@
       </c>
       <c r="I198" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J198" s="24" t="s">
         <v>41</v>
@@ -34854,7 +34854,7 @@
       </c>
       <c r="O198" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P198" s="46" t="s">
         <v>42</v>
@@ -34954,7 +34954,7 @@
       </c>
       <c r="I199" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J199" s="24" t="s">
         <v>41</v>
@@ -34974,7 +34974,7 @@
       </c>
       <c r="O199" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P199" s="46" t="s">
         <v>42</v>
@@ -35074,7 +35074,7 @@
       </c>
       <c r="I200" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J200" s="21" t="s">
         <v>41</v>
@@ -35432,7 +35432,7 @@
       </c>
       <c r="I203" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J203" s="21" t="s">
         <v>41</v>
@@ -36088,7 +36088,7 @@
       </c>
       <c r="I209" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J209" s="20" t="s">
         <v>60</v>
@@ -36279,7 +36279,7 @@
       </c>
       <c r="AF210" s="22" t="str">
         <f t="shared" ca="1" si="45"/>
-        <v>OK!</v>
+        <v>Vence - 60 dias</v>
       </c>
       <c r="AG210" s="45" t="s">
         <v>84</v>
@@ -36332,7 +36332,7 @@
       </c>
       <c r="I211" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J211" s="24" t="s">
         <v>41</v>
@@ -36406,7 +36406,7 @@
       </c>
       <c r="AF211" s="22" t="str">
         <f t="shared" ca="1" si="45"/>
-        <v>Vence - 60 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="AG211" s="45" t="s">
         <v>84</v>
@@ -36585,7 +36585,7 @@
       </c>
       <c r="I213" s="24" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J213" s="20" t="s">
         <v>60</v>
@@ -36859,7 +36859,7 @@
       </c>
       <c r="O215" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P215" s="46" t="s">
         <v>42</v>
@@ -36986,7 +36986,7 @@
       </c>
       <c r="O216" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P216" s="46" t="s">
         <v>42</v>
@@ -37416,7 +37416,7 @@
       </c>
       <c r="AF219" s="22" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AG219" s="45" t="s">
         <v>84</v>
@@ -37723,7 +37723,7 @@
       </c>
       <c r="I222" s="24" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J222" s="24" t="s">
         <v>60</v>
@@ -37797,7 +37797,7 @@
       </c>
       <c r="AF222" s="22" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>Vence - 90 dias</v>
+        <v>Vence - 60 dias</v>
       </c>
       <c r="AG222" s="45" t="s">
         <v>84</v>
@@ -37870,7 +37870,7 @@
       </c>
       <c r="O223" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P223" s="46" t="s">
         <v>42</v>
@@ -38353,7 +38353,7 @@
       </c>
       <c r="I227" s="24" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J227" s="24" t="s">
         <v>41</v>
@@ -39116,7 +39116,7 @@
       </c>
       <c r="O233" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P233" s="46" t="s">
         <v>42</v>
@@ -39237,7 +39237,7 @@
       </c>
       <c r="O234" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P234" s="46" t="s">
         <v>42</v>
@@ -39351,7 +39351,7 @@
       </c>
       <c r="O235" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P235" s="46" t="s">
         <v>42</v>
@@ -39465,7 +39465,7 @@
       </c>
       <c r="O236" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P236" s="46" t="s">
         <v>42</v>
@@ -39579,7 +39579,7 @@
       </c>
       <c r="O237" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P237" s="46" t="s">
         <v>42</v>
@@ -39693,7 +39693,7 @@
       </c>
       <c r="O238" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P238" s="46" t="s">
         <v>42</v>
@@ -39813,7 +39813,7 @@
       </c>
       <c r="O239" s="46" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P239" s="46" t="s">
         <v>42</v>
@@ -40177,7 +40177,7 @@
       </c>
       <c r="I242" s="24" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J242" s="24" t="s">
         <v>60</v>
@@ -40248,7 +40248,7 @@
       </c>
       <c r="AF242" s="22" t="str">
         <f t="shared" ca="1" si="56"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="AG242" s="45" t="s">
         <v>84</v>
@@ -40562,7 +40562,7 @@
       </c>
       <c r="I245" s="24" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J245" s="24" t="s">
         <v>60</v>
@@ -40692,7 +40692,7 @@
       </c>
       <c r="I246" s="24" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J246" s="24" t="s">
         <v>60</v>
@@ -41199,7 +41199,7 @@
       </c>
       <c r="I250" s="24" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J250" s="24" t="s">
         <v>60</v>
@@ -44476,7 +44476,7 @@
       </c>
       <c r="I275" s="24" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J275" s="21" t="s">
         <v>60</v>
@@ -44548,7 +44548,7 @@
       </c>
       <c r="AF275" s="22" t="str">
         <f ca="1">IFERROR(IF(AD275="","?",IF((AD275+(730))&lt;TODAY(),"Vencido",IF((AD275+(365*2))=TODAY(),"Vence Hoje",IF((AD275+(365*2)-15)&lt;=TODAY(),"Vence - 15 dias",IF((AD275+(365*2)-30)&lt;=TODAY(),"Vence - 30 dias",IF((AD275+(365*2)-60)&lt;=TODAY(),"Vence - 60 dias",IF((AD275+(365*2)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AG275" s="45" t="s">
         <v>84</v>
@@ -44806,7 +44806,7 @@
       </c>
       <c r="AF277" s="22" t="str">
         <f ca="1">IFERROR(IF(AD277="","?",IF((AD277+(730))&lt;TODAY(),"Vencido",IF((AD277+(365*2))=TODAY(),"Vence Hoje",IF((AD277+(365*2)-15)&lt;=TODAY(),"Vence - 15 dias",IF((AD277+(365*2)-30)&lt;=TODAY(),"Vence - 30 dias",IF((AD277+(365*2)-60)&lt;=TODAY(),"Vence - 60 dias",IF((AD277+(365*2)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AG277" s="45" t="s">
         <v>84</v>
@@ -45358,7 +45358,7 @@
       </c>
       <c r="I282" s="24" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J282" s="21" t="s">
         <v>60</v>
@@ -45609,7 +45609,7 @@
       </c>
       <c r="I284" s="24" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J284" s="21" t="s">
         <v>60</v>
@@ -45739,7 +45739,7 @@
       </c>
       <c r="I285" s="24" t="str">
         <f t="shared" ref="I285:I300" ca="1" si="68">IFERROR(IF(G285="","?",IF((G285+(365))&lt;TODAY(),"Vencido",IF((G285+(365))=TODAY(),"Vence Hoje",IF((G285+(365)-15)&lt;=TODAY(),"Vence - 15 dias",IF((G285+(365)-30)&lt;=TODAY(),"Vence - 30 dias",IF((G285+(365*2)-60)&lt;=TODAY(),"Vence - 60 dias",IF((G285+(365*2)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J285" s="24" t="s">
         <v>60</v>
@@ -45759,7 +45759,7 @@
       </c>
       <c r="O285" s="46" t="str">
         <f t="shared" ca="1" si="58"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P285" s="46" t="s">
         <v>42</v>
@@ -45883,7 +45883,7 @@
       </c>
       <c r="O286" s="46" t="str">
         <f t="shared" ca="1" si="58"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="P286" s="46" t="s">
         <v>42</v>
@@ -46066,7 +46066,7 @@
       </c>
       <c r="AJ287" s="22" t="str">
         <f t="shared" ca="1" si="67"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AK287" s="33">
         <v>45016</v>
@@ -46193,7 +46193,7 @@
       </c>
       <c r="AJ288" s="22" t="str">
         <f t="shared" ca="1" si="67"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="AK288" s="33">
         <v>45016</v>
@@ -46237,7 +46237,7 @@
       </c>
       <c r="I289" s="24" t="str">
         <f t="shared" ca="1" si="68"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J289" s="21" t="s">
         <v>60</v>
@@ -47464,7 +47464,7 @@
       </c>
       <c r="I298" s="24" t="str">
         <f t="shared" ca="1" si="68"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J298" s="21" t="s">
         <v>41</v>
@@ -51307,7 +51307,7 @@
       </c>
       <c r="I11" s="24" t="str">
         <f t="shared" ref="I11:I34" ca="1" si="5">IFERROR(IF(G11="","?",IF((G11+(365))&lt;TODAY(),"Vencido",IF((G11+(365))=TODAY(),"Vence Hoje",IF((G11+(365)-15)&lt;=TODAY(),"Vence - 15 dias",IF((G11+(365)-30)&lt;=TODAY(),"Vence - 30 dias",IF((G11+(365)-60)&lt;=TODAY(),"Vence - 60 dias",IF((G11+(365)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J11" s="40">
         <v>45122</v>
@@ -51369,7 +51369,7 @@
       </c>
       <c r="I12" s="24" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J12" s="40">
         <v>45122</v>
@@ -52163,7 +52163,7 @@
       </c>
       <c r="I17" s="24" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Vence - 90 dias</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J17" s="77">
         <v>45614</v>
@@ -52513,7 +52513,7 @@
       </c>
       <c r="I21" s="24" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Vence - 90 dias</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J21" s="77">
         <v>45555</v>
@@ -52575,7 +52575,7 @@
       </c>
       <c r="I22" s="24" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J22" s="40">
         <v>45122</v>
@@ -52758,7 +52758,7 @@
       </c>
       <c r="I23" s="24" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Vence - 90 dias</v>
+        <v>Vence - 60 dias</v>
       </c>
       <c r="J23" s="77">
         <v>45562</v>
@@ -52820,7 +52820,7 @@
       </c>
       <c r="I24" s="24" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Vence - 60 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J24" s="40">
         <v>45122</v>
@@ -52995,7 +52995,7 @@
       </c>
       <c r="I26" s="24" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J26" s="40"/>
       <c r="K26" s="40">
@@ -53849,7 +53849,7 @@
       </c>
       <c r="I32" s="24" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Vence - 60 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J32" s="77">
         <v>45519</v>
@@ -53860,7 +53860,7 @@
       </c>
       <c r="L32" s="46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M32" s="21">
         <v>45730</v>
@@ -54032,7 +54032,7 @@
       </c>
       <c r="I33" s="24" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>Vence - 60 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J33" s="77">
         <v>45523</v>
@@ -54043,7 +54043,7 @@
       </c>
       <c r="L33" s="46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M33" s="21">
         <v>45730</v>
@@ -54575,7 +54575,7 @@
       </c>
       <c r="L38" s="46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M38" s="21"/>
       <c r="N38" s="22" t="str">
@@ -54925,7 +54925,7 @@
       </c>
       <c r="L40" s="46" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M40" s="21"/>
       <c r="N40" s="22" t="str">
@@ -58261,7 +58261,7 @@
       </c>
       <c r="I64" s="24" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J64" s="40">
         <v>45538</v>
@@ -59347,7 +59347,7 @@
       </c>
       <c r="I71" s="24" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J71" s="40">
         <v>45194</v>
@@ -60192,7 +60192,7 @@
       </c>
       <c r="I76" s="24" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J76" s="77">
         <v>45527</v>
@@ -63074,7 +63074,7 @@
       </c>
       <c r="L109" s="46" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M109" s="21">
         <v>45664</v>
@@ -63499,7 +63499,7 @@
       </c>
       <c r="I117" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J117" s="40">
         <v>45549</v>
@@ -63517,14 +63517,14 @@
       </c>
       <c r="N117" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O117" s="33">
         <v>45536</v>
       </c>
       <c r="P117" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="Q117" s="60"/>
       <c r="R117" s="40"/>
@@ -63557,7 +63557,7 @@
       </c>
       <c r="I118" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J118" s="40">
         <v>45549</v>
@@ -63575,14 +63575,14 @@
       </c>
       <c r="N118" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O118" s="33">
         <v>45536</v>
       </c>
       <c r="P118" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="Q118" s="60"/>
       <c r="R118" s="40"/>
@@ -63615,7 +63615,7 @@
       </c>
       <c r="I119" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J119" s="40">
         <v>45549</v>
@@ -63633,14 +63633,14 @@
       </c>
       <c r="N119" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O119" s="33">
         <v>45536</v>
       </c>
       <c r="P119" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="Q119" s="60"/>
       <c r="R119" s="40"/>
@@ -63673,7 +63673,7 @@
       </c>
       <c r="I120" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J120" s="40">
         <v>45549</v>
@@ -63691,14 +63691,14 @@
       </c>
       <c r="N120" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O120" s="33">
         <v>45536</v>
       </c>
       <c r="P120" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="Q120" s="60"/>
       <c r="R120" s="40"/>
@@ -63731,7 +63731,7 @@
       </c>
       <c r="I121" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J121" s="40">
         <v>45549</v>
@@ -63749,14 +63749,14 @@
       </c>
       <c r="N121" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O121" s="33">
         <v>45536</v>
       </c>
       <c r="P121" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="Q121" s="60"/>
       <c r="R121" s="40"/>
@@ -63789,7 +63789,7 @@
       </c>
       <c r="I122" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J122" s="40">
         <v>45549</v>
@@ -63807,14 +63807,14 @@
       </c>
       <c r="N122" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O122" s="33">
         <v>45536</v>
       </c>
       <c r="P122" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="Q122" s="60"/>
       <c r="R122" s="40"/>
@@ -63919,14 +63919,14 @@
       </c>
       <c r="N124" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O124" s="33">
         <v>45593</v>
       </c>
       <c r="P124" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="Q124" s="40" t="s">
         <v>85</v>
@@ -63979,14 +63979,14 @@
       </c>
       <c r="N125" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O125" s="33">
         <v>45593</v>
       </c>
       <c r="P125" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="Q125" s="40" t="s">
         <v>85</v>
@@ -64023,7 +64023,7 @@
       </c>
       <c r="I126" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J126" s="40"/>
       <c r="K126" s="40">
@@ -64039,14 +64039,14 @@
       </c>
       <c r="N126" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O126" s="33">
         <v>45593</v>
       </c>
       <c r="P126" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="Q126" s="40" t="s">
         <v>85</v>
@@ -64220,14 +64220,14 @@
       </c>
       <c r="N127" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O127" s="33">
         <v>45593</v>
       </c>
       <c r="P127" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="Q127" s="40" t="s">
         <v>85</v>
@@ -64280,14 +64280,14 @@
       </c>
       <c r="N128" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O128" s="33">
         <v>45593</v>
       </c>
       <c r="P128" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="Q128" s="40" t="s">
         <v>85</v>
@@ -64461,14 +64461,14 @@
       </c>
       <c r="N129" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O129" s="33">
         <v>45593</v>
       </c>
       <c r="P129" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="Q129" s="40" t="s">
         <v>85</v>
@@ -64642,14 +64642,14 @@
       </c>
       <c r="N130" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O130" s="33">
         <v>45593</v>
       </c>
       <c r="P130" s="25" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="Q130" s="40" t="s">
         <v>85</v>
@@ -64704,14 +64704,14 @@
       </c>
       <c r="N131" s="22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Vence - 60 dias</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="O131" s="33">
         <v>45593</v>
       </c>
       <c r="P131" s="25" t="str">
         <f t="shared" ref="P131:P194" ca="1" si="17">IFERROR(IF(O131="","?",IF((O131+(365))&lt;TODAY(),"Vencido",IF((O131+(365))=TODAY(),"Vence Hoje",IF((O131+(365)-15)&lt;=TODAY(),"Vence - 15 dias",IF((O131+(365)-30)&lt;=TODAY(),"Vence - 30 dias",IF((O131+(365)-60)&lt;=TODAY(),"Vence - 60 dias",IF((O131+(365)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="Q131" s="40" t="s">
         <v>85</v>
@@ -65021,7 +65021,7 @@
       </c>
       <c r="I136" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J136" s="77">
         <v>45679</v>
@@ -65135,7 +65135,7 @@
       </c>
       <c r="I138" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J138" s="77">
         <v>45679</v>
@@ -65710,7 +65710,7 @@
       </c>
       <c r="I147" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J147" s="77">
         <v>45525</v>
@@ -65956,7 +65956,7 @@
       </c>
       <c r="I151" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J151" s="40">
         <v>45553</v>
@@ -66018,7 +66018,7 @@
       </c>
       <c r="I152" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J152" s="77">
         <v>45426</v>
@@ -66080,7 +66080,7 @@
       </c>
       <c r="I153" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J153" s="77">
         <v>45428</v>
@@ -66386,7 +66386,7 @@
       </c>
       <c r="I158" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J158" s="77">
         <v>45621</v>
@@ -66411,7 +66411,7 @@
       </c>
       <c r="P158" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q158" s="60" t="s">
         <v>61</v>
@@ -66448,7 +66448,7 @@
       </c>
       <c r="I159" s="24" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J159" s="40">
         <v>45512</v>
@@ -66459,7 +66459,7 @@
       </c>
       <c r="L159" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M159" s="21">
         <v>44958</v>
@@ -66473,7 +66473,7 @@
       </c>
       <c r="P159" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q159" s="60" t="s">
         <v>61</v>
@@ -66701,7 +66701,7 @@
       </c>
       <c r="L163" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M163" s="21">
         <v>45297</v>
@@ -66883,7 +66883,7 @@
       </c>
       <c r="L166" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M166" s="21">
         <v>45297</v>
@@ -67782,7 +67782,7 @@
       </c>
       <c r="I181" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J181" s="77">
         <v>45637</v>
@@ -67840,7 +67840,7 @@
       </c>
       <c r="I182" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J182" s="77">
         <v>45511</v>
@@ -67851,7 +67851,7 @@
       </c>
       <c r="L182" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M182" s="21"/>
       <c r="N182" s="22" t="str">
@@ -67863,7 +67863,7 @@
       </c>
       <c r="P182" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q182" s="60" t="s">
         <v>84</v>
@@ -67911,7 +67911,7 @@
       </c>
       <c r="L183" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M183" s="21"/>
       <c r="N183" s="22" t="str">
@@ -67923,7 +67923,7 @@
       </c>
       <c r="P183" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q183" s="60" t="s">
         <v>84</v>
@@ -67971,7 +67971,7 @@
       </c>
       <c r="L184" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M184" s="21"/>
       <c r="N184" s="22" t="str">
@@ -67983,7 +67983,7 @@
       </c>
       <c r="P184" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q184" s="60" t="s">
         <v>84</v>
@@ -68031,7 +68031,7 @@
       </c>
       <c r="L185" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M185" s="21"/>
       <c r="N185" s="22" t="str">
@@ -68043,7 +68043,7 @@
       </c>
       <c r="P185" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q185" s="60" t="s">
         <v>84</v>
@@ -68091,7 +68091,7 @@
       </c>
       <c r="L186" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M186" s="21"/>
       <c r="N186" s="22" t="str">
@@ -68103,7 +68103,7 @@
       </c>
       <c r="P186" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q186" s="60" t="s">
         <v>84</v>
@@ -68140,7 +68140,7 @@
       </c>
       <c r="I187" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J187" s="77">
         <v>45518</v>
@@ -68151,7 +68151,7 @@
       </c>
       <c r="L187" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M187" s="21"/>
       <c r="N187" s="22" t="str">
@@ -68163,7 +68163,7 @@
       </c>
       <c r="P187" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q187" s="60" t="s">
         <v>90</v>
@@ -68200,7 +68200,7 @@
       </c>
       <c r="I188" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J188" s="40"/>
       <c r="K188" s="40">
@@ -68221,7 +68221,7 @@
       </c>
       <c r="P188" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q188" s="60" t="s">
         <v>85</v>
@@ -68258,7 +68258,7 @@
       </c>
       <c r="I189" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J189" s="77">
         <v>45511</v>
@@ -68269,7 +68269,7 @@
       </c>
       <c r="L189" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M189" s="21"/>
       <c r="N189" s="22" t="str">
@@ -68281,7 +68281,7 @@
       </c>
       <c r="P189" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q189" s="60" t="s">
         <v>84</v>
@@ -68329,7 +68329,7 @@
       </c>
       <c r="L190" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M190" s="21"/>
       <c r="N190" s="22" t="str">
@@ -68341,7 +68341,7 @@
       </c>
       <c r="P190" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q190" s="60" t="s">
         <v>84</v>
@@ -68401,7 +68401,7 @@
       </c>
       <c r="P191" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q191" s="60" t="s">
         <v>84</v>
@@ -68459,7 +68459,7 @@
       </c>
       <c r="P192" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q192" s="60" t="s">
         <v>84</v>
@@ -68507,7 +68507,7 @@
       </c>
       <c r="L193" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M193" s="21"/>
       <c r="N193" s="22" t="str">
@@ -68519,7 +68519,7 @@
       </c>
       <c r="P193" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q193" s="60" t="s">
         <v>84</v>
@@ -68567,7 +68567,7 @@
       </c>
       <c r="L194" s="46" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M194" s="21"/>
       <c r="N194" s="22" t="str">
@@ -68579,7 +68579,7 @@
       </c>
       <c r="P194" s="25" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q194" s="60" t="s">
         <v>85</v>
@@ -68627,7 +68627,7 @@
       </c>
       <c r="L195" s="46" t="str">
         <f t="shared" ref="L195:L259" ca="1" si="23">IFERROR(IF(J195="","?",IF((J195+(365))&lt;TODAY(),"Bloqueado",IF((J195+(365*2))=TODAY(),"Vence Hoje",IF((J195+(365*2)-15)&lt;=TODAY(),"Vence - 15 dias",IF((J195+(365*2)-30)&lt;=TODAY(),"Vence - 30 dias",IF((J195+(365*2)-60)&lt;=TODAY(),"Vence - 60 dias",IF((J195+(365*2)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M195" s="21"/>
       <c r="N195" s="22" t="str">
@@ -68639,7 +68639,7 @@
       </c>
       <c r="P195" s="25" t="str">
         <f t="shared" ref="P195:P258" ca="1" si="24">IFERROR(IF(O195="","?",IF((O195+(365))&lt;TODAY(),"Vencido",IF((O195+(365))=TODAY(),"Vence Hoje",IF((O195+(365)-15)&lt;=TODAY(),"Vence - 15 dias",IF((O195+(365)-30)&lt;=TODAY(),"Vence - 30 dias",IF((O195+(365)-60)&lt;=TODAY(),"Vence - 60 dias",IF((O195+(365)-90)&lt;=TODAY(),"Vence - 90 dias","OK!"))))))),"-")</f>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q195" s="60" t="s">
         <v>85</v>
@@ -68927,7 +68927,7 @@
       </c>
       <c r="L200" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M200" s="21"/>
       <c r="N200" s="22" t="str">
@@ -68939,7 +68939,7 @@
       </c>
       <c r="P200" s="25" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="Q200" s="60" t="s">
         <v>61</v>
@@ -68976,7 +68976,7 @@
       </c>
       <c r="I201" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J201" s="77">
         <v>45583</v>
@@ -69034,7 +69034,7 @@
       </c>
       <c r="I202" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J202" s="77">
         <v>45583</v>
@@ -69092,7 +69092,7 @@
       </c>
       <c r="I203" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J203" s="77">
         <v>45582</v>
@@ -69223,7 +69223,7 @@
       </c>
       <c r="L205" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M205" s="21"/>
       <c r="N205" s="22" t="str">
@@ -69268,7 +69268,7 @@
       </c>
       <c r="I206" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J206" s="77">
         <v>45517</v>
@@ -69279,7 +69279,7 @@
       </c>
       <c r="L206" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M206" s="21"/>
       <c r="N206" s="22" t="str">
@@ -69326,7 +69326,7 @@
       </c>
       <c r="I207" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J207" s="77">
         <v>45518</v>
@@ -69337,7 +69337,7 @@
       </c>
       <c r="L207" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M207" s="21"/>
       <c r="N207" s="22" t="str">
@@ -69440,7 +69440,7 @@
       </c>
       <c r="I209" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J209" s="77">
         <v>45520</v>
@@ -69451,7 +69451,7 @@
       </c>
       <c r="L209" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M209" s="21"/>
       <c r="N209" s="22" t="str">
@@ -69498,7 +69498,7 @@
       </c>
       <c r="I210" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vencido</v>
       </c>
       <c r="J210" s="77">
         <v>45518</v>
@@ -69509,7 +69509,7 @@
       </c>
       <c r="L210" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M210" s="21"/>
       <c r="N210" s="22" t="str">
@@ -69846,7 +69846,7 @@
       </c>
       <c r="I216" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J216" s="77">
         <v>45635</v>
@@ -69960,7 +69960,7 @@
       </c>
       <c r="I218" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J218" s="77">
         <v>45552</v>
@@ -70076,7 +70076,7 @@
       </c>
       <c r="I220" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J220" s="77">
         <v>45618</v>
@@ -70203,7 +70203,7 @@
       </c>
       <c r="L222" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M222" s="21"/>
       <c r="N222" s="22" t="str">
@@ -70261,7 +70261,7 @@
       </c>
       <c r="L223" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M223" s="21"/>
       <c r="N223" s="22" t="str">
@@ -70596,7 +70596,7 @@
       </c>
       <c r="I229" s="24" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J229" s="77">
         <v>45552</v>
@@ -70665,7 +70665,7 @@
       </c>
       <c r="L230" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M230" s="21"/>
       <c r="N230" s="22" t="str">
@@ -70883,7 +70883,7 @@
       </c>
       <c r="I234" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J234" s="77">
         <v>45546</v>
@@ -71236,7 +71236,7 @@
       </c>
       <c r="L240" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M240" s="21"/>
       <c r="N240" s="22" t="str">
@@ -71294,7 +71294,7 @@
       </c>
       <c r="L241" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M241" s="21"/>
       <c r="N241" s="22" t="str">
@@ -71352,7 +71352,7 @@
       </c>
       <c r="L242" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M242" s="21"/>
       <c r="N242" s="22" t="str">
@@ -71410,7 +71410,7 @@
       </c>
       <c r="L243" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M243" s="21"/>
       <c r="N243" s="22" t="str">
@@ -71468,7 +71468,7 @@
       </c>
       <c r="L244" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M244" s="21"/>
       <c r="N244" s="22" t="str">
@@ -71526,7 +71526,7 @@
       </c>
       <c r="L245" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M245" s="21"/>
       <c r="N245" s="22" t="str">
@@ -71584,7 +71584,7 @@
       </c>
       <c r="L246" s="46" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M246" s="21">
         <v>45292</v>
@@ -71757,7 +71757,7 @@
       </c>
       <c r="I249" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J249" s="77">
         <v>45526</v>
@@ -71943,7 +71943,7 @@
       </c>
       <c r="I252" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J252" s="77">
         <v>45551</v>
@@ -72005,7 +72005,7 @@
       </c>
       <c r="I253" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>Vence - 15 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J253" s="77">
         <v>45530</v>
@@ -72248,7 +72248,7 @@
       </c>
       <c r="I257" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J257" s="77">
         <v>45807</v>
@@ -73717,7 +73717,7 @@
       </c>
       <c r="I279" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Vence - 15 dias</v>
       </c>
       <c r="J279" s="40"/>
       <c r="K279" s="40">
@@ -73837,7 +73837,7 @@
       </c>
       <c r="I281" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J281" s="77">
         <v>45685</v>
@@ -73899,7 +73899,7 @@
       </c>
       <c r="I282" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J282" s="77">
         <v>45513</v>
@@ -73910,7 +73910,7 @@
       </c>
       <c r="L282" s="46" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M282" s="21">
         <v>45292</v>
@@ -73972,7 +73972,7 @@
       </c>
       <c r="L283" s="46" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>OK!</v>
+        <v>Bloqueado</v>
       </c>
       <c r="M283" s="21">
         <v>45292</v>
@@ -74039,7 +74039,7 @@
       </c>
       <c r="N284" s="22" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="O284" s="33">
         <v>45016</v>
@@ -74099,7 +74099,7 @@
       </c>
       <c r="N285" s="22" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>OK!</v>
+        <v>Vence - 90 dias</v>
       </c>
       <c r="O285" s="33">
         <v>45016</v>
@@ -74143,7 +74143,7 @@
       </c>
       <c r="I286" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>OK!</v>
+        <v>Vence - 30 dias</v>
       </c>
       <c r="J286" s="40"/>
       <c r="K286" s="40">
@@ -74713,7 +74713,7 @@
       </c>
       <c r="I294" s="24" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>Vence - 30 dias</v>
+        <v>Vencido</v>
       </c>
       <c r="J294" s="77">
         <v>45729</v>
@@ -76975,12 +76975,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6393da93-b5d4-43d4-9fc9-7527d55b015d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -77166,17 +77165,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6393da93-b5d4-43d4-9fc9-7527d55b015d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8B27588-8D45-4E77-91FE-8E14105FCF15}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26BD5D32-4838-46AB-9B7C-9396A25C222C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6393da93-b5d4-43d4-9fc9-7527d55b015d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -77200,11 +77202,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26BD5D32-4838-46AB-9B7C-9396A25C222C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8B27588-8D45-4E77-91FE-8E14105FCF15}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6393da93-b5d4-43d4-9fc9-7527d55b015d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>